<commit_message>
Updated programmatically generated v5 spreadsheet template to include all latest modules
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/v5/template/Programmatically_generated_v5_template_spreadsheet.xlsx
+++ b/examples/spreadsheets/v5/template/Programmatically_generated_v5_template_spreadsheet.xlsx
@@ -2,7 +2,6 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
@@ -21,8 +20,9 @@
     <sheet name="enrichment_process" sheetId="12" state="visible" r:id="rId12"/>
     <sheet name="library_preparation_process" sheetId="13" state="visible" r:id="rId13"/>
     <sheet name="sequencing_process" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet name="sequence_file" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="purchased_reagents" sheetId="15" state="visible" r:id="rId15"/>
     <sheet name="protocol" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="sequence_file" sheetId="17" state="visible" r:id="rId17"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -30,9 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="240">
-  <si>
-    <t>A unique ID for the project.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="343">
+  <si>
+    <t>A unique label for the project.</t>
   </si>
   <si>
     <t>A summary of the project in a sentence.</t>
@@ -59,16 +59,19 @@
     <t>A list of other projects that may be logically grouped with this one.</t>
   </si>
   <si>
-    <t>A title of a grant proposal, publication, or poster. Approximately 30 words.</t>
-  </si>
-  <si>
-    <t>An abstract from a grant application, publication, or poster. Approximately 300 words.</t>
+    <t>Tissue Stability</t>
+  </si>
+  <si>
+    <t>A title of a grant proposal or publication. Approximately 30 words.</t>
+  </si>
+  <si>
+    <t>An abstract from a grant application or publication. Approximately 300 words.</t>
   </si>
   <si>
     <t>Experimental design documents, electronic notebook files, manuscripts in preparation, etc.</t>
   </si>
   <si>
-    <t>Project ID</t>
+    <t>Project shortname</t>
   </si>
   <si>
     <t>Project title</t>
@@ -110,6 +113,9 @@
     <t>A URL, preferably not behind a paywall, for the publication.</t>
   </si>
   <si>
+    <t>Shortname for project this publication relates to</t>
+  </si>
+  <si>
     <t>Smith JD</t>
   </si>
   <si>
@@ -155,6 +161,9 @@
     <t>Country where contact works.</t>
   </si>
   <si>
+    <t>Shortname for project this contact relates to</t>
+  </si>
+  <si>
     <t>John,D,Doe</t>
   </si>
   <si>
@@ -212,6 +221,12 @@
     <t>The body mass index of the organism.</t>
   </si>
   <si>
+    <t>An array of ontology terms from EMBL-EBI's Ancestry Ontology describing ancestral groups, uncategorised ancestral groups, and population isolates.</t>
+  </si>
+  <si>
+    <t>The name of the strain.</t>
+  </si>
+  <si>
     <t>Cause of death from death report for human donor, from research lab for mouse.</t>
   </si>
   <si>
@@ -227,27 +242,75 @@
     <t>Date and time of death of the organism, in format yyyy-mm-ddThh:mm:ssZ.</t>
   </si>
   <si>
+    <t>Number of drinks consumed on a typical day.</t>
+  </si>
+  <si>
+    <t>List of medications the organism was currently taking at time of biomaterial donation.</t>
+  </si>
+  <si>
+    <t>Should be one of normal, fasting, or feeding tube removed.</t>
+  </si>
+  <si>
+    <t>Estimated number of cigarettes smoked per day and for how many years.</t>
+  </si>
+  <si>
+    <t>Results from any medical tests performed on the individual.</t>
+  </si>
+  <si>
+    <t>Any treatments the individual has undergone.</t>
+  </si>
+  <si>
+    <t>The scientific binomial name for the species of the biomaterial.</t>
+  </si>
+  <si>
     <t>Age in age_units. Measured since birth.</t>
   </si>
   <si>
+    <t>The unit in which age is expressed. Must be one of hour, day, week, month, or year.</t>
+  </si>
+  <si>
+    <t>A classification of the developmental stage of the organism.</t>
+  </si>
+  <si>
+    <t>Short description of disease status of the organism.</t>
+  </si>
+  <si>
     <t>Gestational age in gestational_age_units. Measured since fertilization.</t>
   </si>
   <si>
-    <t>Height of organism in meters.</t>
+    <t>The unit in which gestational age is expressed. Must be one of hour, day, week, month, or year.</t>
+  </si>
+  <si>
+    <t>Height of organism in height units.</t>
+  </si>
+  <si>
+    <t>The unit in which height is expressed. Must be a child term of https://www.ebi.ac.uk/ols/ontologies/uo/terms?iri=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FUO_0000001.</t>
   </si>
   <si>
     <t>Yes if organism is living at time of biomaterial collection. No otherwise.</t>
   </si>
   <si>
-    <t>Sex of organism. Should be one of male, female, mixed, or unknown.</t>
+    <t>The biological sex of the organism. Should be one of male, female, mixed, or unknown.</t>
   </si>
   <si>
     <t>Weight of organism in kilograms.</t>
   </si>
   <si>
+    <t>The unit in which weight is expressed. Must be a child term of https://www.ebi.ac.uk/ols/ontologies/uo/terms?iri=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FUO_0000002.</t>
+  </si>
+  <si>
     <t>IDs of processes for which this biomaterial is an input</t>
   </si>
   <si>
+    <t>C57BL/6.</t>
+  </si>
+  <si>
+    <t>Homo sapiens</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
     <t>Biomaterial ID</t>
   </si>
   <si>
@@ -278,6 +341,12 @@
     <t>Body mass index</t>
   </si>
   <si>
+    <t>Ethnicity</t>
+  </si>
+  <si>
+    <t>Strain</t>
+  </si>
+  <si>
     <t>Cause of death</t>
   </si>
   <si>
@@ -293,15 +362,51 @@
     <t>Time of death</t>
   </si>
   <si>
+    <t>Alcohol history</t>
+  </si>
+  <si>
+    <t>Medications</t>
+  </si>
+  <si>
+    <t>Nutritional state</t>
+  </si>
+  <si>
+    <t>Smoking history</t>
+  </si>
+  <si>
+    <t>Test results</t>
+  </si>
+  <si>
+    <t>Treatments</t>
+  </si>
+  <si>
+    <t>Genus species</t>
+  </si>
+  <si>
     <t>Organism age</t>
   </si>
   <si>
+    <t>Organism age unit</t>
+  </si>
+  <si>
+    <t>Development stage</t>
+  </si>
+  <si>
+    <t>Disease</t>
+  </si>
+  <si>
     <t>Gestational age</t>
   </si>
   <si>
+    <t>Gestational age unit</t>
+  </si>
+  <si>
     <t>Height</t>
   </si>
   <si>
+    <t>Height unit</t>
+  </si>
+  <si>
     <t>Is living?</t>
   </si>
   <si>
@@ -311,6 +416,9 @@
     <t>Weight</t>
   </si>
   <si>
+    <t>Weight unit</t>
+  </si>
+  <si>
     <t>Process IDs</t>
   </si>
   <si>
@@ -323,6 +431,9 @@
     <t>This organism is a sibling of the indicated organism.</t>
   </si>
   <si>
+    <t>ID for biomaterial this familial_relationship relates to</t>
+  </si>
+  <si>
     <t>Child of</t>
   </si>
   <si>
@@ -332,6 +443,15 @@
     <t>Sibling of</t>
   </si>
   <si>
+    <t>The organ that the biomaterial came from. Blood and connective tissue are considered organs.</t>
+  </si>
+  <si>
+    <t>A term for a specific part of the organ that the biomaterial came from.</t>
+  </si>
+  <si>
+    <t>Short description of disease status of the specimen. Can be 'normal' or one or more disease terms.</t>
+  </si>
+  <si>
     <t>State of tissue breakdown due to self-digestion. Must be one of: none, mild, moderate.</t>
   </si>
   <si>
@@ -356,7 +476,34 @@
     <t>Duration of time, in seconds, between when death is declared and when the tissue is preserved or processed.</t>
   </si>
   <si>
-    <t>When the biomaterial was collection, in date-time format, yyyy-mm-ddThh:mm:ssZ.</t>
+    <t>The method by which a biomaterial was stored.</t>
+  </si>
+  <si>
+    <t>Length of time the biomaterial was stored for in Storage time units.</t>
+  </si>
+  <si>
+    <t>The unit in which Storage time is expressed.</t>
+  </si>
+  <si>
+    <t>The method by which a biomaterial was preserved or not.</t>
+  </si>
+  <si>
+    <t>When the biomaterial was collected, in date-time format, yyyy-mm-ddThh:mm:ssZ.</t>
+  </si>
+  <si>
+    <t>Blood</t>
+  </si>
+  <si>
+    <t>Umbilical cord blood</t>
+  </si>
+  <si>
+    <t>days</t>
+  </si>
+  <si>
+    <t>Organ</t>
+  </si>
+  <si>
+    <t>Organ part</t>
   </si>
   <si>
     <t>Autolysis score</t>
@@ -383,6 +530,15 @@
     <t>Post-mortem interval</t>
   </si>
   <si>
+    <t>Storage method</t>
+  </si>
+  <si>
+    <t>Storage time</t>
+  </si>
+  <si>
+    <t>Storage time unit</t>
+  </si>
+  <si>
     <t>Time of collection</t>
   </si>
   <si>
@@ -392,6 +548,9 @@
     <t>The size of the cells. Average cell size is acceptable.</t>
   </si>
   <si>
+    <t>The unit in which the cell size is expressed. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/uo/terms?iri=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FUO_0000001.</t>
+  </si>
+  <si>
     <t>Percent of cells determined to be viable.</t>
   </si>
   <si>
@@ -401,15 +560,48 @@
     <t>Percent of cells identified to be necrotic.</t>
   </si>
   <si>
+    <t>The number of passages the cell line has been through.</t>
+  </si>
+  <si>
+    <t>The solid, liquid, or semi-solid medium used to support the growth of the biomaterial.</t>
+  </si>
+  <si>
+    <t>The method used for detecting mycoplasma contamination of a biomaterial culture.</t>
+  </si>
+  <si>
+    <t>Results of mycoplasma testing of a biomaterial culture.</t>
+  </si>
+  <si>
+    <t>Description of drugs added to the growth medium for this biomaterial.</t>
+  </si>
+  <si>
+    <t>Cell types expected to be present in the suspension. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/clo/terms?iri=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FCL_0000003.</t>
+  </si>
+  <si>
     <t>Total estimated number of cells in biomaterial. May be 1 for well-based assays.</t>
   </si>
   <si>
+    <t>lysogeny broth (LB) medium</t>
+  </si>
+  <si>
+    <t>Indirect DNA stain using Hoechst 33258 with 3T3 indicator cells</t>
+  </si>
+  <si>
+    <t>No spots of bright blue stain observed at high magnification</t>
+  </si>
+  <si>
+    <t>100 ug/mL ampicillin</t>
+  </si>
+  <si>
     <t>Cell morphology</t>
   </si>
   <si>
     <t>Cell size number</t>
   </si>
   <si>
+    <t>Cell size unit</t>
+  </si>
+  <si>
     <t>Percent cell viability</t>
   </si>
   <si>
@@ -419,6 +611,24 @@
     <t>Percent necrosis</t>
   </si>
   <si>
+    <t>Passage number</t>
+  </si>
+  <si>
+    <t>Growth medium</t>
+  </si>
+  <si>
+    <t>Mycoplasma testing method</t>
+  </si>
+  <si>
+    <t>Mycoplasma testing results</t>
+  </si>
+  <si>
+    <t>Drug treatment</t>
+  </si>
+  <si>
+    <t>Target cell type</t>
+  </si>
+  <si>
     <t>Total estimated cell count</t>
   </si>
   <si>
@@ -428,13 +638,19 @@
     <t>The supplier catalogue URL for the cell line.</t>
   </si>
   <si>
+    <t>The cell cycle phase if the cell line is synchronized growing cells or the phase is known. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/go/terms?iri=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FGO_0007049.</t>
+  </si>
+  <si>
     <t>The type of cell line. Must be one of primary, immortalized, stem cell-derived, or synthetic.</t>
   </si>
   <si>
+    <t>The cell type that the cell line was derived from. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/clo/terms?iri=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FCL_0000003.</t>
+  </si>
+  <si>
     <t>When the cell line was established, in date-time format. yyyy-mm-ddThh:mm:ssZ.</t>
   </si>
   <si>
-    <t>The number of passages the cell line has been through.</t>
+    <t>Free text describing any disease association to the cell type. Should be an EFO ontology.</t>
   </si>
   <si>
     <t>Catalog number</t>
@@ -443,24 +659,39 @@
     <t>Catalog URL</t>
   </si>
   <si>
+    <t>Cell cycle</t>
+  </si>
+  <si>
     <t>Cell line type</t>
   </si>
   <si>
+    <t>Cell type</t>
+  </si>
+  <si>
     <t>Date established</t>
   </si>
   <si>
-    <t>Passage number</t>
+    <t>Organ for which this organoid is a model system.</t>
   </si>
   <si>
     <t>Age of the organoid.</t>
   </si>
   <si>
+    <t>The unit in which organoid age is expressed. Must be one of hour, day, week, month, or year.</t>
+  </si>
+  <si>
     <t>The type of organoid. Must be one of primary, immortalized, stem cell-derived, or synthetic.</t>
   </si>
   <si>
+    <t>Organ model</t>
+  </si>
+  <si>
     <t>Organoid age</t>
   </si>
   <si>
+    <t>Organoid age unit</t>
+  </si>
+  <si>
     <t>Organoid type</t>
   </si>
   <si>
@@ -479,7 +710,10 @@
     <t>Where the process took place.</t>
   </si>
   <si>
-    <t>Name of the individual(s) who executed this process.</t>
+    <t>Identifier for individual(s) who executed this process.</t>
+  </si>
+  <si>
+    <t>The type of process. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/efo/terms?iri=http%3A%2F%2Fwww.ebi.ac.uk%2Fefo%2FEFO_0002694.</t>
   </si>
   <si>
     <t>How the biomaterial was collected.</t>
@@ -494,7 +728,7 @@
     <t>Wellcome Sanger Institute, Teichman Lab.</t>
   </si>
   <si>
-    <t>John Smith||Jane Doe</t>
+    <t>Technician 1</t>
   </si>
   <si>
     <t>Process ID</t>
@@ -512,7 +746,10 @@
     <t>Location</t>
   </si>
   <si>
-    <t>Researcher</t>
+    <t>Operator identity</t>
+  </si>
+  <si>
+    <t>Process type</t>
   </si>
   <si>
     <t>Collection method</t>
@@ -533,16 +770,16 @@
     <t>Nucleic acid source</t>
   </si>
   <si>
-    <t>How enrichment was achieved.</t>
+    <t>The method by which enrichment was achieved.</t>
   </si>
   <si>
     <t>A space-delimited list of markers with +/-.</t>
   </si>
   <si>
-    <t>Minimum size passing selection in microns.</t>
-  </si>
-  <si>
-    <t>Maximum size passing selection in microns.</t>
+    <t>Minimum cell or organelle size passing selection, in microns.</t>
+  </si>
+  <si>
+    <t>Maximum cell or organelle size passing selection, in microns.</t>
   </si>
   <si>
     <t>FACS</t>
@@ -551,16 +788,16 @@
     <t>CD4+ CD8-</t>
   </si>
   <si>
-    <t>Enrichment type</t>
+    <t>Enrichment method</t>
   </si>
   <si>
     <t>Markers</t>
   </si>
   <si>
-    <t>Minimum size</t>
-  </si>
-  <si>
-    <t>Maximum size</t>
+    <t>Minimum size selected</t>
+  </si>
+  <si>
+    <t>Maximum size selected</t>
   </si>
   <si>
     <t>The read that the barcode is found in. Should be one of Read 1, Read 2, i7 Index, or i5 Index.</t>
@@ -575,6 +812,9 @@
     <t>Name of file containing legitimate barcode sequences.</t>
   </si>
   <si>
+    <t>Specific type of nucleic acid molecule from which a sequencing library was prepared. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/efo/terms?iri=http%3A%2F%2Fwww.ebi.ac.uk%2Fefo%2FEFO_0004446.</t>
+  </si>
+  <si>
     <t>The general approach for sequencing library construction.</t>
   </si>
   <si>
@@ -587,10 +827,10 @@
     <t>Library strandedness.</t>
   </si>
   <si>
-    <t>Name of RNA spike-in kit.</t>
-  </si>
-  <si>
-    <t>Dilution of RNA spike-in.</t>
+    <t>Name of spike-in kit.</t>
+  </si>
+  <si>
+    <t>Dilution of spike-in.</t>
   </si>
   <si>
     <t>Smart-seq2</t>
@@ -614,6 +854,9 @@
     <t>Cell White list barcode file</t>
   </si>
   <si>
+    <t>Input molecule</t>
+  </si>
+  <si>
     <t>Library construction approach</t>
   </si>
   <si>
@@ -644,6 +887,9 @@
     <t>UMI White list barcode file</t>
   </si>
   <si>
+    <t>The manufacturer and model of the sequencer used. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/efo/terms?iri=http%3A%2F%2Fwww.ebi.ac.uk%2Fefo%2FEFO_0000548.</t>
+  </si>
+  <si>
     <t>Local name for the particular machine on which the biomaterial was sequenced.</t>
   </si>
   <si>
@@ -656,6 +902,12 @@
     <t>An INSDC (International Nucleotide Sequence Database Collaboration) run accession. Accession must start with DRR, ERR, or SRR.</t>
   </si>
   <si>
+    <t>Illumina HiSeq 4000</t>
+  </si>
+  <si>
+    <t>Instrument manufacturer and model</t>
+  </si>
+  <si>
     <t>Local machine name</t>
   </si>
   <si>
@@ -668,6 +920,99 @@
     <t>INSDC run</t>
   </si>
   <si>
+    <t>The retail name of the kit/reagent.</t>
+  </si>
+  <si>
+    <t>The catalog number of the kit/reagent.</t>
+  </si>
+  <si>
+    <t>The manufacturer of the kit/reagent.</t>
+  </si>
+  <si>
+    <t>The batch or lot number of the kit/reagent.</t>
+  </si>
+  <si>
+    <t>The date of expiration for the kit/reagent.</t>
+  </si>
+  <si>
+    <t>ID for process this purchased_reagents relates to</t>
+  </si>
+  <si>
+    <t>SureCell WTA 3' Library Prep Kit</t>
+  </si>
+  <si>
+    <t>20014279</t>
+  </si>
+  <si>
+    <t>Illumina</t>
+  </si>
+  <si>
+    <t>10001A</t>
+  </si>
+  <si>
+    <t>2018-01-31</t>
+  </si>
+  <si>
+    <t>Retail name</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Batch/lot number</t>
+  </si>
+  <si>
+    <t>Expiry date</t>
+  </si>
+  <si>
+    <t>A unique ID for this protocol.</t>
+  </si>
+  <si>
+    <t>A short, descriptive name for the protocol that need not be unique.</t>
+  </si>
+  <si>
+    <t>A general description of the protocol.</t>
+  </si>
+  <si>
+    <t>The publication digital object identifier (doi) associated with the protocol.</t>
+  </si>
+  <si>
+    <t>The protocols.io digital object identifier (doi) associated with the protocol.</t>
+  </si>
+  <si>
+    <t>A filename of a PDF document containing the details of the protocol.</t>
+  </si>
+  <si>
+    <t>The type of protocol. Must be a child term of https://www.ebi.ac.uk/ols/ontologies/efo/terms?iri=http%3A%2F%2Fpurl.obolibrary.org%2Fobo%2FOBI_0000272.</t>
+  </si>
+  <si>
+    <t>10.1101/193219</t>
+  </si>
+  <si>
+    <t>10.17504/protocols.io.mgjc3un</t>
+  </si>
+  <si>
+    <t>Protocol ID</t>
+  </si>
+  <si>
+    <t>Protocol name</t>
+  </si>
+  <si>
+    <t>Protocol description</t>
+  </si>
+  <si>
+    <t>Publication DOI</t>
+  </si>
+  <si>
+    <t>protocols.io DOI</t>
+  </si>
+  <si>
+    <t>Document filename</t>
+  </si>
+  <si>
+    <t>Protocol type</t>
+  </si>
+  <si>
     <t>The filename of the data file.</t>
   </si>
   <si>
@@ -677,19 +1022,22 @@
     <t>MD5 checksum of the data file.</t>
   </si>
   <si>
-    <t>Whether the read represents the r1, r2, i1, or i2 part of the sequencing read.</t>
+    <t>Whether the read file contains the read1, read2, index1, or index2 part of the sequencing read. If read file represents a single-end, non-indexed library, indicate that here.</t>
   </si>
   <si>
     <t>The index of the lane that this file was sequenced from.</t>
   </si>
   <si>
+    <t>The length of a sequenced read in this file, in nucleotides.</t>
+  </si>
+  <si>
     <t>ID of the biomaterial to which this file relates</t>
   </si>
   <si>
     <t>ID of the sequencing process to which this file relates</t>
   </si>
   <si>
-    <t>r1</t>
+    <t>read1</t>
   </si>
   <si>
     <t>File name</t>
@@ -707,49 +1055,10 @@
     <t>Lane index</t>
   </si>
   <si>
+    <t>Read length</t>
+  </si>
+  <si>
     <t>Sequencing process ID</t>
-  </si>
-  <si>
-    <t>A unique ID for this protocol.</t>
-  </si>
-  <si>
-    <t>A short, descriptive name for the protocol that need not be unique.</t>
-  </si>
-  <si>
-    <t>A general description of the protocol.</t>
-  </si>
-  <si>
-    <t>The publication digital object identifier (doi) associated with the protocol.</t>
-  </si>
-  <si>
-    <t>A filename of a PDF containing the details of the protocol.</t>
-  </si>
-  <si>
-    <t>The retail name of the protocol kit used.</t>
-  </si>
-  <si>
-    <t>The batch of protocol kit used.</t>
-  </si>
-  <si>
-    <t>SureCell WTA 3' Library Prep Kit</t>
-  </si>
-  <si>
-    <t>Protocol ID</t>
-  </si>
-  <si>
-    <t>Protocol name</t>
-  </si>
-  <si>
-    <t>Protocol description</t>
-  </si>
-  <si>
-    <t>PDF</t>
-  </si>
-  <si>
-    <t>Retail name</t>
-  </si>
-  <si>
-    <t>Batch number</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1408,18 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="17"/>
+    <col customWidth="1" max="2" min="2" width="13"/>
+    <col customWidth="1" max="3" min="3" width="19"/>
+    <col customWidth="1" max="4" min="4" width="19"/>
+    <col customWidth="1" max="5" min="5" width="23"/>
+    <col customWidth="1" max="6" min="6" width="20"/>
+    <col customWidth="1" max="7" min="7" width="22"/>
+    <col customWidth="1" max="8" min="8" width="21"/>
+    <col customWidth="1" max="9" min="9" width="16"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -1131,15 +1451,17 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="1" t="n"/>
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E2" s="1" t="n"/>
       <c r="F2" s="1" t="n"/>
@@ -1149,31 +1471,31 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1187,80 +1509,98 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
+    <col customWidth="1" max="3" min="3" width="19"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="8"/>
+    <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="12"/>
+    <col customWidth="1" max="8" min="8" width="17"/>
+    <col customWidth="1" max="9" min="9" width="12"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F1" t="s">
-        <v>149</v>
+        <v>226</v>
       </c>
       <c r="G1" t="s">
-        <v>150</v>
+        <v>227</v>
       </c>
       <c r="H1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>228</v>
+      </c>
+      <c r="I1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>153</v>
+        <v>231</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>154</v>
+        <v>232</v>
       </c>
       <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>234</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>236</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>159</v>
+        <v>237</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>161</v>
+        <v>239</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>162</v>
+        <v>240</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -1274,87 +1614,106 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
+    <col customWidth="1" max="3" min="3" width="19"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="8"/>
+    <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="19"/>
+    <col customWidth="1" max="8" min="8" width="19"/>
+    <col customWidth="1" max="9" min="9" width="12"/>
+    <col customWidth="1" max="10" min="10" width="12"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F1" t="s">
-        <v>149</v>
+        <v>226</v>
       </c>
       <c r="G1" t="s">
-        <v>163</v>
+        <v>242</v>
       </c>
       <c r="H1" t="s">
-        <v>164</v>
+        <v>243</v>
       </c>
       <c r="I1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+        <v>227</v>
+      </c>
+      <c r="J1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>153</v>
+        <v>231</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>154</v>
+        <v>232</v>
       </c>
       <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="n"/>
       <c r="I2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>234</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>236</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>159</v>
+        <v>237</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>165</v>
+        <v>244</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>166</v>
+        <v>245</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>162</v>
+        <v>239</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -1368,105 +1727,126 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
+    <col customWidth="1" max="3" min="3" width="19"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="8"/>
+    <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="17"/>
+    <col customWidth="1" max="8" min="8" width="7"/>
+    <col customWidth="1" max="9" min="9" width="21"/>
+    <col customWidth="1" max="10" min="10" width="21"/>
+    <col customWidth="1" max="11" min="11" width="12"/>
+    <col customWidth="1" max="12" min="12" width="12"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F1" t="s">
-        <v>149</v>
+        <v>226</v>
       </c>
       <c r="G1" t="s">
-        <v>167</v>
+        <v>246</v>
       </c>
       <c r="H1" t="s">
-        <v>168</v>
+        <v>247</v>
       </c>
       <c r="I1" t="s">
-        <v>169</v>
+        <v>248</v>
       </c>
       <c r="J1" t="s">
-        <v>170</v>
+        <v>249</v>
       </c>
       <c r="K1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>227</v>
+      </c>
+      <c r="L1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>153</v>
+        <v>231</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>154</v>
+        <v>232</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>171</v>
+        <v>250</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>172</v>
+        <v>251</v>
       </c>
       <c r="I2" s="1" t="n"/>
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>234</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>236</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>159</v>
+        <v>237</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>173</v>
+        <v>252</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>174</v>
+        <v>253</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>175</v>
+        <v>254</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>176</v>
+        <v>255</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>162</v>
+        <v>239</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -1480,177 +1860,216 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:W3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
+    <col customWidth="1" max="3" min="3" width="19"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="8"/>
+    <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="28"/>
+    <col customWidth="1" max="8" min="8" width="19"/>
+    <col customWidth="1" max="9" min="9" width="19"/>
+    <col customWidth="1" max="10" min="10" width="28"/>
+    <col customWidth="1" max="11" min="11" width="14"/>
+    <col customWidth="1" max="12" min="12" width="29"/>
+    <col customWidth="1" max="13" min="13" width="8"/>
+    <col customWidth="1" max="14" min="14" width="6"/>
+    <col customWidth="1" max="15" min="15" width="6"/>
+    <col customWidth="1" max="16" min="16" width="12"/>
+    <col customWidth="1" max="17" min="17" width="17"/>
+    <col customWidth="1" max="18" min="18" width="27"/>
+    <col customWidth="1" max="19" min="19" width="18"/>
+    <col customWidth="1" max="20" min="20" width="18"/>
+    <col customWidth="1" max="21" min="21" width="27"/>
+    <col customWidth="1" max="22" min="22" width="12"/>
+    <col customWidth="1" max="23" min="23" width="12"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F1" t="s">
-        <v>149</v>
+        <v>226</v>
       </c>
       <c r="G1" t="s">
-        <v>177</v>
+        <v>256</v>
       </c>
       <c r="H1" t="s">
-        <v>178</v>
+        <v>257</v>
       </c>
       <c r="I1" t="s">
-        <v>179</v>
+        <v>258</v>
       </c>
       <c r="J1" t="s">
-        <v>180</v>
+        <v>259</v>
       </c>
       <c r="K1" t="s">
-        <v>181</v>
+        <v>260</v>
       </c>
       <c r="L1" t="s">
-        <v>182</v>
+        <v>261</v>
       </c>
       <c r="M1" t="s">
-        <v>183</v>
+        <v>262</v>
       </c>
       <c r="N1" t="s">
-        <v>184</v>
+        <v>263</v>
       </c>
       <c r="O1" t="s">
-        <v>185</v>
+        <v>264</v>
       </c>
       <c r="P1" t="s">
-        <v>186</v>
+        <v>265</v>
       </c>
       <c r="Q1" t="s">
-        <v>177</v>
+        <v>266</v>
       </c>
       <c r="R1" t="s">
-        <v>178</v>
+        <v>256</v>
       </c>
       <c r="S1" t="s">
-        <v>179</v>
+        <v>257</v>
       </c>
       <c r="T1" t="s">
-        <v>180</v>
+        <v>258</v>
       </c>
       <c r="U1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
+        <v>259</v>
+      </c>
+      <c r="V1" t="s">
+        <v>227</v>
+      </c>
+      <c r="W1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>153</v>
+        <v>231</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>154</v>
+        <v>232</v>
       </c>
       <c r="G2" s="1" t="n"/>
       <c r="H2" s="1" t="n"/>
       <c r="I2" s="1" t="n"/>
       <c r="J2" s="1" t="n"/>
-      <c r="K2" s="1" t="s">
-        <v>187</v>
-      </c>
+      <c r="K2" s="1" t="n"/>
       <c r="L2" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="M2" s="1" t="n"/>
+        <v>267</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="N2" s="1" t="n"/>
-      <c r="O2" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="P2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="Q2" s="1" t="n"/>
       <c r="R2" s="1" t="n"/>
       <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="n"/>
       <c r="U2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="V2" s="1" t="n"/>
+      <c r="W2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>234</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>236</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>159</v>
+        <v>237</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>190</v>
+        <v>270</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>191</v>
+        <v>271</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>192</v>
+        <v>272</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>193</v>
+        <v>273</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>194</v>
+        <v>274</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>195</v>
+        <v>275</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>196</v>
+        <v>276</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>197</v>
+        <v>277</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>198</v>
+        <v>278</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>199</v>
+        <v>279</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>200</v>
+        <v>280</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>201</v>
+        <v>281</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>202</v>
+        <v>282</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>203</v>
+        <v>283</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>162</v>
+        <v>284</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -1664,101 +2083,132 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="12"/>
+    <col customWidth="1" max="3" min="3" width="19"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="8"/>
+    <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="33"/>
+    <col customWidth="1" max="8" min="8" width="18"/>
+    <col customWidth="1" max="9" min="9" width="12"/>
+    <col customWidth="1" max="10" min="10" width="16"/>
+    <col customWidth="1" max="11" min="11" width="9"/>
+    <col customWidth="1" max="12" min="12" width="12"/>
+    <col customWidth="1" max="13" min="13" width="12"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>221</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>222</v>
       </c>
       <c r="C1" t="s">
-        <v>146</v>
+        <v>223</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>224</v>
       </c>
       <c r="E1" t="s">
-        <v>148</v>
+        <v>225</v>
       </c>
       <c r="F1" t="s">
-        <v>149</v>
+        <v>226</v>
       </c>
       <c r="G1" t="s">
-        <v>204</v>
+        <v>285</v>
       </c>
       <c r="H1" t="s">
-        <v>205</v>
+        <v>286</v>
       </c>
       <c r="I1" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="J1" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="K1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>289</v>
+      </c>
+      <c r="L1" t="s">
+        <v>227</v>
+      </c>
+      <c r="M1" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>152</v>
+        <v>230</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>153</v>
+        <v>231</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="G2" s="1" t="n"/>
+        <v>232</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>290</v>
+      </c>
       <c r="H2" s="1" t="n"/>
       <c r="I2" s="1" t="n"/>
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>156</v>
+        <v>234</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>157</v>
+        <v>235</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>158</v>
+        <v>236</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>159</v>
+        <v>237</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>160</v>
+        <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>208</v>
+        <v>291</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>210</v>
+        <v>293</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>211</v>
+        <v>294</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>162</v>
+        <v>295</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -1772,71 +2222,78 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="11"/>
+    <col customWidth="1" max="2" min="2" width="14"/>
+    <col customWidth="1" max="3" min="3" width="12"/>
+    <col customWidth="1" max="4" min="4" width="16"/>
+    <col customWidth="1" max="5" min="5" width="11"/>
+    <col customWidth="1" max="6" min="6" width="10"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>212</v>
+        <v>296</v>
       </c>
       <c r="B1" t="s">
-        <v>213</v>
+        <v>297</v>
       </c>
       <c r="C1" t="s">
-        <v>214</v>
+        <v>298</v>
       </c>
       <c r="D1" t="s">
-        <v>215</v>
+        <v>299</v>
       </c>
       <c r="E1" t="s">
-        <v>216</v>
+        <v>300</v>
       </c>
       <c r="F1" t="s">
-        <v>217</v>
-      </c>
-      <c r="G1" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1" t="n"/>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>304</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>1</v>
+        <v>305</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>220</v>
+        <v>307</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>222</v>
+        <v>308</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>223</v>
+        <v>309</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>224</v>
+        <v>310</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>225</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1856,29 +2313,38 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="11"/>
+    <col customWidth="1" max="2" min="2" width="13"/>
+    <col customWidth="1" max="3" min="3" width="20"/>
+    <col customWidth="1" max="4" min="4" width="15"/>
+    <col customWidth="1" max="5" min="5" width="16"/>
+    <col customWidth="1" max="6" min="6" width="17"/>
+    <col customWidth="1" max="7" min="7" width="13"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>226</v>
+        <v>311</v>
       </c>
       <c r="B1" t="s">
-        <v>227</v>
+        <v>312</v>
       </c>
       <c r="C1" t="s">
-        <v>228</v>
+        <v>313</v>
       </c>
       <c r="D1" t="s">
-        <v>229</v>
+        <v>314</v>
       </c>
       <c r="E1" t="s">
-        <v>230</v>
+        <v>315</v>
       </c>
       <c r="F1" t="s">
-        <v>231</v>
+        <v>316</v>
       </c>
       <c r="G1" t="s">
-        <v>232</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1886,35 +2352,132 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="1" t="n"/>
-      <c r="F2" s="1" t="s">
-        <v>233</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="F2" s="1" t="n"/>
       <c r="G2" s="1" t="n"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>234</v>
+        <v>320</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>235</v>
+        <v>321</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>236</v>
+        <v>322</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>31</v>
+        <v>323</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>237</v>
+        <v>324</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>238</v>
+        <v>325</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>239</v>
+        <v>326</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="9"/>
+    <col customWidth="1" max="2" min="2" width="11"/>
+    <col customWidth="1" max="3" min="3" width="8"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="10"/>
+    <col customWidth="1" max="6" min="6" width="11"/>
+    <col customWidth="1" max="7" min="7" width="14"/>
+    <col customWidth="1" max="8" min="8" width="21"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>327</v>
+      </c>
+      <c r="B1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D1" t="s">
+        <v>330</v>
+      </c>
+      <c r="E1" t="s">
+        <v>331</v>
+      </c>
+      <c r="F1" t="s">
+        <v>332</v>
+      </c>
+      <c r="G1" t="s">
+        <v>333</v>
+      </c>
+      <c r="H1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -1934,60 +2497,68 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="7"/>
+    <col customWidth="1" max="2" min="2" width="17"/>
+    <col customWidth="1" max="3" min="3" width="5"/>
+    <col customWidth="1" max="4" min="4" width="5"/>
+    <col customWidth="1" max="5" min="5" width="15"/>
+    <col customWidth="1" max="6" min="6" width="17"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="n"/>
       <c r="F2" s="1" t="n"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2007,37 +2578,47 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="12"/>
+    <col customWidth="1" max="2" min="2" width="5"/>
+    <col customWidth="1" max="3" min="3" width="12"/>
+    <col customWidth="1" max="4" min="4" width="11"/>
+    <col customWidth="1" max="5" min="5" width="10"/>
+    <col customWidth="1" max="6" min="6" width="7"/>
+    <col customWidth="1" max="7" min="7" width="7"/>
+    <col customWidth="1" max="8" min="8" width="17"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H1" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
@@ -2049,28 +2630,28 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2084,86 +2665,1033 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:AL3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="14"/>
+    <col customWidth="1" max="2" min="2" width="16"/>
+    <col customWidth="1" max="3" min="3" width="23"/>
+    <col customWidth="1" max="4" min="4" width="13"/>
+    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="6" min="6" width="8"/>
+    <col customWidth="1" max="7" min="7" width="9"/>
+    <col customWidth="1" max="8" min="8" width="19"/>
+    <col customWidth="1" max="9" min="9" width="12"/>
+    <col customWidth="1" max="10" min="10" width="8"/>
+    <col customWidth="1" max="11" min="11" width="15"/>
+    <col customWidth="1" max="12" min="12" width="9"/>
+    <col customWidth="1" max="13" min="13" width="6"/>
+    <col customWidth="1" max="14" min="14" width="14"/>
+    <col customWidth="1" max="15" min="15" width="14"/>
+    <col customWidth="1" max="16" min="16" width="28"/>
+    <col customWidth="1" max="17" min="17" width="20"/>
+    <col customWidth="1" max="18" min="18" width="13"/>
+    <col customWidth="1" max="19" min="19" width="15"/>
+    <col customWidth="1" max="20" min="20" width="11"/>
+    <col customWidth="1" max="21" min="21" width="17"/>
+    <col customWidth="1" max="22" min="22" width="15"/>
+    <col customWidth="1" max="23" min="23" width="12"/>
+    <col customWidth="1" max="24" min="24" width="10"/>
+    <col customWidth="1" max="25" min="25" width="13"/>
+    <col customWidth="1" max="26" min="26" width="12"/>
+    <col customWidth="1" max="27" min="27" width="17"/>
+    <col customWidth="1" max="28" min="28" width="17"/>
+    <col customWidth="1" max="29" min="29" width="7"/>
+    <col customWidth="1" max="30" min="30" width="15"/>
+    <col customWidth="1" max="31" min="31" width="20"/>
+    <col customWidth="1" max="32" min="32" width="6"/>
+    <col customWidth="1" max="33" min="33" width="11"/>
+    <col customWidth="1" max="34" min="34" width="10"/>
+    <col customWidth="1" max="35" min="35" width="14"/>
+    <col customWidth="1" max="36" min="36" width="6"/>
+    <col customWidth="1" max="37" min="37" width="11"/>
+    <col customWidth="1" max="38" min="38" width="11"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:38">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M1" t="s">
+        <v>64</v>
+      </c>
+      <c r="N1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O1" t="s">
+        <v>66</v>
+      </c>
+      <c r="P1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" t="s">
+        <v>71</v>
+      </c>
+      <c r="U1" t="s">
+        <v>72</v>
+      </c>
+      <c r="V1" t="s">
+        <v>73</v>
+      </c>
+      <c r="W1" t="s">
+        <v>74</v>
+      </c>
+      <c r="X1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>84</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+      <c r="K2" s="1" t="n"/>
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
+      <c r="R2" s="1" t="n"/>
+      <c r="S2" s="1" t="n"/>
+      <c r="T2" s="1" t="n"/>
+      <c r="U2" s="1" t="n"/>
+      <c r="V2" s="1" t="n"/>
+      <c r="W2" s="1" t="n"/>
+      <c r="X2" s="1" t="n"/>
+      <c r="Y2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z2" s="1" t="n"/>
+      <c r="AA2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="AB2" s="1" t="n"/>
+      <c r="AC2" s="1" t="n"/>
+      <c r="AD2" s="1" t="n"/>
+      <c r="AE2" s="1" t="n"/>
+      <c r="AF2" s="1" t="n"/>
+      <c r="AG2" s="1" t="n"/>
+      <c r="AH2" s="1" t="n"/>
+      <c r="AI2" s="1" t="n"/>
+      <c r="AJ2" s="1" t="n"/>
+      <c r="AK2" s="1" t="n"/>
+      <c r="AL2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:38">
+      <c r="A3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL3" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="8"/>
+    <col customWidth="1" max="2" min="2" width="9"/>
+    <col customWidth="1" max="3" min="3" width="10"/>
+    <col customWidth="1" max="4" min="4" width="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AB3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="14"/>
+    <col customWidth="1" max="2" min="2" width="16"/>
+    <col customWidth="1" max="3" min="3" width="23"/>
+    <col customWidth="1" max="4" min="4" width="13"/>
+    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="6" min="6" width="8"/>
+    <col customWidth="1" max="7" min="7" width="9"/>
+    <col customWidth="1" max="8" min="8" width="19"/>
+    <col customWidth="1" max="9" min="9" width="12"/>
+    <col customWidth="1" max="10" min="10" width="8"/>
+    <col customWidth="1" max="11" min="11" width="13"/>
+    <col customWidth="1" max="12" min="12" width="5"/>
+    <col customWidth="1" max="13" min="13" width="10"/>
+    <col customWidth="1" max="14" min="14" width="7"/>
+    <col customWidth="1" max="15" min="15" width="15"/>
+    <col customWidth="1" max="16" min="16" width="17"/>
+    <col customWidth="1" max="17" min="17" width="11"/>
+    <col customWidth="1" max="18" min="18" width="20"/>
+    <col customWidth="1" max="19" min="19" width="13"/>
+    <col customWidth="1" max="20" min="20" width="23"/>
+    <col customWidth="1" max="21" min="21" width="17"/>
+    <col customWidth="1" max="22" min="22" width="20"/>
+    <col customWidth="1" max="23" min="23" width="14"/>
+    <col customWidth="1" max="24" min="24" width="12"/>
+    <col customWidth="1" max="25" min="25" width="17"/>
+    <col customWidth="1" max="26" min="26" width="14"/>
+    <col customWidth="1" max="27" min="27" width="18"/>
+    <col customWidth="1" max="28" min="28" width="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" t="s">
         <v>52</v>
       </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
       <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L1" t="s">
+        <v>137</v>
+      </c>
+      <c r="M1" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O1" t="s">
+        <v>140</v>
+      </c>
+      <c r="P1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>142</v>
+      </c>
+      <c r="R1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S1" t="s">
+        <v>144</v>
+      </c>
+      <c r="T1" t="s">
+        <v>145</v>
+      </c>
+      <c r="U1" t="s">
+        <v>146</v>
+      </c>
+      <c r="V1" t="s">
+        <v>147</v>
+      </c>
+      <c r="W1" t="s">
+        <v>148</v>
+      </c>
+      <c r="X1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>150</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+      <c r="K2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
+      <c r="R2" s="1" t="n"/>
+      <c r="S2" s="1" t="n"/>
+      <c r="T2" s="1" t="n"/>
+      <c r="U2" s="1" t="n"/>
+      <c r="V2" s="1" t="n"/>
+      <c r="W2" s="1" t="n"/>
+      <c r="X2" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z2" s="1" t="n"/>
+      <c r="AA2" s="1" t="n"/>
+      <c r="AB2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:28">
+      <c r="A3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Y3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="14"/>
+    <col customWidth="1" max="2" min="2" width="16"/>
+    <col customWidth="1" max="3" min="3" width="23"/>
+    <col customWidth="1" max="4" min="4" width="13"/>
+    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="6" min="6" width="8"/>
+    <col customWidth="1" max="7" min="7" width="9"/>
+    <col customWidth="1" max="8" min="8" width="19"/>
+    <col customWidth="1" max="9" min="9" width="12"/>
+    <col customWidth="1" max="10" min="10" width="8"/>
+    <col customWidth="1" max="11" min="11" width="15"/>
+    <col customWidth="1" max="12" min="12" width="16"/>
+    <col customWidth="1" max="13" min="13" width="14"/>
+    <col customWidth="1" max="14" min="14" width="22"/>
+    <col customWidth="1" max="15" min="15" width="21"/>
+    <col customWidth="1" max="16" min="16" width="16"/>
+    <col customWidth="1" max="17" min="17" width="14"/>
+    <col customWidth="1" max="18" min="18" width="13"/>
+    <col customWidth="1" max="19" min="19" width="25"/>
+    <col customWidth="1" max="20" min="20" width="26"/>
+    <col customWidth="1" max="21" min="21" width="14"/>
+    <col customWidth="1" max="22" min="22" width="13"/>
+    <col customWidth="1" max="23" min="23" width="16"/>
+    <col customWidth="1" max="24" min="24" width="26"/>
+    <col customWidth="1" max="25" min="25" width="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
       <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M1" t="s">
+        <v>172</v>
+      </c>
+      <c r="N1" t="s">
+        <v>173</v>
+      </c>
+      <c r="O1" t="s">
+        <v>174</v>
+      </c>
+      <c r="P1" t="s">
+        <v>175</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>176</v>
+      </c>
+      <c r="R1" t="s">
+        <v>177</v>
+      </c>
+      <c r="S1" t="s">
+        <v>178</v>
+      </c>
+      <c r="T1" t="s">
+        <v>179</v>
+      </c>
+      <c r="U1" t="s">
+        <v>180</v>
+      </c>
+      <c r="V1" t="s">
+        <v>76</v>
+      </c>
+      <c r="W1" t="s">
+        <v>181</v>
+      </c>
+      <c r="X1" t="s">
+        <v>182</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="1" t="n"/>
+      <c r="C2" s="1" t="n"/>
+      <c r="D2" s="1" t="n"/>
+      <c r="E2" s="1" t="n"/>
+      <c r="F2" s="1" t="n"/>
+      <c r="G2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+      <c r="K2" s="1" t="n"/>
+      <c r="L2" s="1" t="n"/>
+      <c r="M2" s="1" t="n"/>
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
+      <c r="R2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="1" t="n"/>
+      <c r="X2" s="1" t="n"/>
+      <c r="Y2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:25">
+      <c r="A3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AD3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="14"/>
+    <col customWidth="1" max="2" min="2" width="16"/>
+    <col customWidth="1" max="3" min="3" width="23"/>
+    <col customWidth="1" max="4" min="4" width="13"/>
+    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="6" min="6" width="8"/>
+    <col customWidth="1" max="7" min="7" width="9"/>
+    <col customWidth="1" max="8" min="8" width="19"/>
+    <col customWidth="1" max="9" min="9" width="12"/>
+    <col customWidth="1" max="10" min="10" width="8"/>
+    <col customWidth="1" max="11" min="11" width="14"/>
+    <col customWidth="1" max="12" min="12" width="11"/>
+    <col customWidth="1" max="13" min="13" width="10"/>
+    <col customWidth="1" max="14" min="14" width="14"/>
+    <col customWidth="1" max="15" min="15" width="15"/>
+    <col customWidth="1" max="16" min="16" width="16"/>
+    <col customWidth="1" max="17" min="17" width="14"/>
+    <col customWidth="1" max="18" min="18" width="22"/>
+    <col customWidth="1" max="19" min="19" width="21"/>
+    <col customWidth="1" max="20" min="20" width="16"/>
+    <col customWidth="1" max="21" min="21" width="14"/>
+    <col customWidth="1" max="22" min="22" width="13"/>
+    <col customWidth="1" max="23" min="23" width="25"/>
+    <col customWidth="1" max="24" min="24" width="26"/>
+    <col customWidth="1" max="25" min="25" width="14"/>
+    <col customWidth="1" max="26" min="26" width="9"/>
+    <col customWidth="1" max="27" min="27" width="16"/>
+    <col customWidth="1" max="28" min="28" width="7"/>
+    <col customWidth="1" max="29" min="29" width="13"/>
+    <col customWidth="1" max="30" min="30" width="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
         <v>54</v>
       </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K1" t="s">
-        <v>59</v>
+        <v>200</v>
       </c>
       <c r="L1" t="s">
-        <v>60</v>
+        <v>201</v>
       </c>
       <c r="M1" t="s">
-        <v>61</v>
+        <v>202</v>
       </c>
       <c r="N1" t="s">
-        <v>62</v>
+        <v>203</v>
       </c>
       <c r="O1" t="s">
-        <v>63</v>
+        <v>170</v>
       </c>
       <c r="P1" t="s">
-        <v>64</v>
+        <v>171</v>
       </c>
       <c r="Q1" t="s">
-        <v>65</v>
+        <v>172</v>
       </c>
       <c r="R1" t="s">
-        <v>66</v>
+        <v>173</v>
       </c>
       <c r="S1" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="T1" t="s">
-        <v>68</v>
+        <v>175</v>
       </c>
       <c r="U1" t="s">
-        <v>69</v>
+        <v>176</v>
       </c>
       <c r="V1" t="s">
-        <v>70</v>
+        <v>177</v>
       </c>
       <c r="W1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
+        <v>178</v>
+      </c>
+      <c r="X1" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>205</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
@@ -2185,78 +3713,116 @@
       <c r="S2" s="1" t="n"/>
       <c r="T2" s="1" t="n"/>
       <c r="U2" s="1" t="n"/>
-      <c r="V2" s="1" t="n"/>
-      <c r="W2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:23">
+      <c r="V2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z2" s="1" t="n"/>
+      <c r="AA2" s="1" t="n"/>
+      <c r="AB2" s="1" t="n"/>
+      <c r="AC2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AD2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:30">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>81</v>
+        <v>207</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>82</v>
+        <v>208</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>83</v>
+        <v>209</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>84</v>
+        <v>210</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>86</v>
+        <v>188</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>87</v>
+        <v>189</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>88</v>
+        <v>190</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>89</v>
+        <v>191</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>90</v>
+        <v>192</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>91</v>
+        <v>193</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>92</v>
+        <v>194</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>93</v>
+        <v>195</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -2264,136 +3830,133 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="14"/>
+    <col customWidth="1" max="2" min="2" width="16"/>
+    <col customWidth="1" max="3" min="3" width="23"/>
+    <col customWidth="1" max="4" min="4" width="13"/>
+    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="6" min="6" width="8"/>
+    <col customWidth="1" max="7" min="7" width="9"/>
+    <col customWidth="1" max="8" min="8" width="19"/>
+    <col customWidth="1" max="9" min="9" width="12"/>
+    <col customWidth="1" max="10" min="10" width="8"/>
+    <col customWidth="1" max="11" min="11" width="15"/>
+    <col customWidth="1" max="12" min="12" width="16"/>
+    <col customWidth="1" max="13" min="13" width="14"/>
+    <col customWidth="1" max="14" min="14" width="22"/>
+    <col customWidth="1" max="15" min="15" width="21"/>
+    <col customWidth="1" max="16" min="16" width="16"/>
+    <col customWidth="1" max="17" min="17" width="14"/>
+    <col customWidth="1" max="18" min="18" width="13"/>
+    <col customWidth="1" max="19" min="19" width="25"/>
+    <col customWidth="1" max="20" min="20" width="26"/>
+    <col customWidth="1" max="21" min="21" width="14"/>
+    <col customWidth="1" max="22" min="22" width="13"/>
+    <col customWidth="1" max="23" min="23" width="11"/>
+    <col customWidth="1" max="24" min="24" width="12"/>
+    <col customWidth="1" max="25" min="25" width="17"/>
+    <col customWidth="1" max="26" min="26" width="13"/>
+    <col customWidth="1" max="27" min="27" width="11"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>54</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="n"/>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:T3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="G1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="I1" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="J1" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="K1" t="s">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="L1" t="s">
-        <v>101</v>
+        <v>171</v>
       </c>
       <c r="M1" t="s">
-        <v>102</v>
+        <v>172</v>
       </c>
       <c r="N1" t="s">
-        <v>103</v>
+        <v>173</v>
       </c>
       <c r="O1" t="s">
-        <v>104</v>
+        <v>174</v>
       </c>
       <c r="P1" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="Q1" t="s">
-        <v>106</v>
+        <v>176</v>
       </c>
       <c r="R1" t="s">
-        <v>107</v>
+        <v>177</v>
       </c>
       <c r="S1" t="s">
-        <v>108</v>
+        <v>178</v>
       </c>
       <c r="T1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
+        <v>179</v>
+      </c>
+      <c r="U1" t="s">
+        <v>180</v>
+      </c>
+      <c r="V1" t="s">
+        <v>76</v>
+      </c>
+      <c r="W1" t="s">
+        <v>213</v>
+      </c>
+      <c r="X1" t="s">
+        <v>214</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>215</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>216</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
@@ -2411,537 +3974,110 @@
       <c r="O2" s="1" t="n"/>
       <c r="P2" s="1" t="n"/>
       <c r="Q2" s="1" t="n"/>
-      <c r="R2" s="1" t="n"/>
-      <c r="S2" s="1" t="n"/>
-      <c r="T2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:20">
+      <c r="R2" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="W2" s="1" t="n"/>
+      <c r="X2" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="1" t="n"/>
+      <c r="Z2" s="1" t="n"/>
+      <c r="AA2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:27">
       <c r="A3" s="2" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>109</v>
+        <v>187</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>111</v>
+        <v>189</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>112</v>
+        <v>190</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>113</v>
+        <v>191</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>114</v>
+        <v>192</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>115</v>
+        <v>193</v>
       </c>
       <c r="R3" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="S3" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:Q3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" t="s">
-        <v>122</v>
-      </c>
-      <c r="P1" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="1" t="n"/>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="n"/>
-      <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-      <c r="H2" s="1" t="n"/>
-      <c r="I2" s="1" t="n"/>
-      <c r="J2" s="1" t="n"/>
-      <c r="K2" s="1" t="n"/>
-      <c r="L2" s="1" t="n"/>
-      <c r="M2" s="1" t="n"/>
-      <c r="N2" s="1" t="n"/>
-      <c r="O2" s="1" t="n"/>
-      <c r="P2" s="1" t="n"/>
-      <c r="Q2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="P3" s="2" t="s">
+      <c r="W3" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="AA3" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:U3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" t="s">
-        <v>130</v>
-      </c>
-      <c r="L1" t="s">
-        <v>131</v>
-      </c>
-      <c r="M1" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" t="s">
-        <v>118</v>
-      </c>
-      <c r="O1" t="s">
-        <v>119</v>
-      </c>
-      <c r="P1" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>121</v>
-      </c>
-      <c r="R1" t="s">
-        <v>122</v>
-      </c>
-      <c r="S1" t="s">
-        <v>133</v>
-      </c>
-      <c r="T1" t="s">
-        <v>134</v>
-      </c>
-      <c r="U1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="1" t="n"/>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="n"/>
-      <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-      <c r="H2" s="1" t="n"/>
-      <c r="I2" s="1" t="n"/>
-      <c r="J2" s="1" t="n"/>
-      <c r="K2" s="1" t="n"/>
-      <c r="L2" s="1" t="n"/>
-      <c r="M2" s="1" t="n"/>
-      <c r="N2" s="1" t="n"/>
-      <c r="O2" s="1" t="n"/>
-      <c r="P2" s="1" t="n"/>
-      <c r="Q2" s="1" t="n"/>
-      <c r="R2" s="1" t="n"/>
-      <c r="S2" s="1" t="n"/>
-      <c r="T2" s="1" t="n"/>
-      <c r="U2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:R3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" t="s">
-        <v>58</v>
-      </c>
-      <c r="K1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" t="s">
-        <v>122</v>
-      </c>
-      <c r="P1" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>141</v>
-      </c>
-      <c r="R1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="1" t="n"/>
-      <c r="B2" s="1" t="n"/>
-      <c r="C2" s="1" t="n"/>
-      <c r="D2" s="1" t="n"/>
-      <c r="E2" s="1" t="n"/>
-      <c r="F2" s="1" t="n"/>
-      <c r="G2" s="1" t="n"/>
-      <c r="H2" s="1" t="n"/>
-      <c r="I2" s="1" t="n"/>
-      <c r="J2" s="1" t="n"/>
-      <c r="K2" s="1" t="n"/>
-      <c r="L2" s="1" t="n"/>
-      <c r="M2" s="1" t="n"/>
-      <c r="N2" s="1" t="n"/>
-      <c r="O2" s="1" t="n"/>
-      <c r="P2" s="1" t="n"/>
-      <c r="Q2" s="1" t="n"/>
-      <c r="R2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated template spreadsheet and docs
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/v5/template/Programmatically_generated_v5_template_spreadsheet.xlsx
+++ b/examples/spreadsheets/v5/template/Programmatically_generated_v5_template_spreadsheet.xlsx
@@ -2,6 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="352">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -323,7 +324,7 @@
     <t>NCBI taxon ID</t>
   </si>
   <si>
-    <t>Derived from</t>
+    <t>Input biomaterial ID</t>
   </si>
   <si>
     <t>Genotype</t>
@@ -812,22 +813,34 @@
     <t>Name of file containing legitimate barcode sequences.</t>
   </si>
   <si>
-    <t>Specific type of nucleic acid molecule from which a sequencing library was prepared. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/efo/terms?iri=http%3A%2F%2Fwww.ebi.ac.uk%2Fefo%2FEFO_0004446.</t>
+    <t>Starting nucleic acid molecule isolated for sequencing. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/efo/terms?iri=http%3A%2F%2Fwww.ebi.ac.uk%2Fefo%2FEFO_0004446.</t>
   </si>
   <si>
     <t>The general approach for sequencing library construction.</t>
   </si>
   <si>
-    <t>The type of end bias the library has. Must be one of 3' bias, 5' bias, 3' end, 5' end, or none.</t>
+    <t>The retail name of the kit/reagent.</t>
+  </si>
+  <si>
+    <t>The catalog number of the kit/reagent.</t>
+  </si>
+  <si>
+    <t>The manufacturer of the kit/reagent.</t>
+  </si>
+  <si>
+    <t>The batch or lot number of the kit/reagent.</t>
+  </si>
+  <si>
+    <t>The date of expiration for the kit/reagent.</t>
+  </si>
+  <si>
+    <t>The type of tag or end bias the library has. Must be one of 3 prime tag, 3 prime end bias, 5 prime tag, 5 prime end bias, or full length.</t>
   </si>
   <si>
     <t>Primer used for cDNA synthesis from RNA. Must be either poly-dT or random.</t>
   </si>
   <si>
-    <t>Library strandedness.</t>
-  </si>
-  <si>
-    <t>Name of spike-in kit.</t>
+    <t>Library strandedness. Must be one of first, second, or unstranded.</t>
   </si>
   <si>
     <t>Dilution of spike-in.</t>
@@ -836,10 +849,25 @@
     <t>Smart-seq2</t>
   </si>
   <si>
-    <t>three_prime_bias</t>
-  </si>
-  <si>
-    <t>ERCC</t>
+    <t>SureCell WTA 3' Library Prep Kit</t>
+  </si>
+  <si>
+    <t>20014279</t>
+  </si>
+  <si>
+    <t>Illumina</t>
+  </si>
+  <si>
+    <t>10001A</t>
+  </si>
+  <si>
+    <t>2018-01-31</t>
+  </si>
+  <si>
+    <t>3_prime_tag</t>
+  </si>
+  <si>
+    <t>unstranded</t>
   </si>
   <si>
     <t>Cell Barcode-containing read</t>
@@ -854,12 +882,24 @@
     <t>Cell White list barcode file</t>
   </si>
   <si>
-    <t>Input molecule</t>
+    <t>Input nucleic acid molecule</t>
   </si>
   <si>
     <t>Library construction approach</t>
   </si>
   <si>
+    <t>Retail name</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Batch/lot number</t>
+  </si>
+  <si>
+    <t>Expiry date</t>
+  </si>
+  <si>
     <t>End bias</t>
   </si>
   <si>
@@ -869,9 +909,6 @@
     <t>Strand</t>
   </si>
   <si>
-    <t>Spike-in kit</t>
-  </si>
-  <si>
     <t>Spike-in dilution</t>
   </si>
   <si>
@@ -902,9 +939,27 @@
     <t>An INSDC (International Nucleotide Sequence Database Collaboration) run accession. Accession must start with DRR, ERR, or SRR.</t>
   </si>
   <si>
+    <t>An ID for the plate that the well is located on.</t>
+  </si>
+  <si>
+    <t>A name for the well. Should be unique for the plate</t>
+  </si>
+  <si>
+    <t>Well row in plate.</t>
+  </si>
+  <si>
+    <t>Well column in plate.</t>
+  </si>
+  <si>
+    <t>Note on how good cell looks if imaged in well before sequencing.</t>
+  </si>
+  <si>
     <t>Illumina HiSeq 4000</t>
   </si>
   <si>
+    <t>yes</t>
+  </si>
+  <si>
     <t>Instrument manufacturer and model</t>
   </si>
   <si>
@@ -920,49 +975,22 @@
     <t>INSDC run</t>
   </si>
   <si>
-    <t>The retail name of the kit/reagent.</t>
-  </si>
-  <si>
-    <t>The catalog number of the kit/reagent.</t>
-  </si>
-  <si>
-    <t>The manufacturer of the kit/reagent.</t>
-  </si>
-  <si>
-    <t>The batch or lot number of the kit/reagent.</t>
-  </si>
-  <si>
-    <t>The date of expiration for the kit/reagent.</t>
+    <t>Well plate ID</t>
+  </si>
+  <si>
+    <t>Well name</t>
+  </si>
+  <si>
+    <t>Well row</t>
+  </si>
+  <si>
+    <t>Well column</t>
+  </si>
+  <si>
+    <t>Cell quality</t>
   </si>
   <si>
     <t>ID for process this purchased_reagents relates to</t>
-  </si>
-  <si>
-    <t>SureCell WTA 3' Library Prep Kit</t>
-  </si>
-  <si>
-    <t>20014279</t>
-  </si>
-  <si>
-    <t>Illumina</t>
-  </si>
-  <si>
-    <t>10001A</t>
-  </si>
-  <si>
-    <t>2018-01-31</t>
-  </si>
-  <si>
-    <t>Retail name</t>
-  </si>
-  <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>Batch/lot number</t>
-  </si>
-  <si>
-    <t>Expiry date</t>
   </si>
   <si>
     <t>A unique ID for this protocol.</t>
@@ -1860,7 +1888,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W3"/>
+  <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1878,22 +1906,36 @@
     <col customWidth="1" max="8" min="8" width="19"/>
     <col customWidth="1" max="9" min="9" width="19"/>
     <col customWidth="1" max="10" min="10" width="28"/>
-    <col customWidth="1" max="11" min="11" width="14"/>
+    <col customWidth="1" max="11" min="11" width="27"/>
     <col customWidth="1" max="12" min="12" width="29"/>
-    <col customWidth="1" max="13" min="13" width="8"/>
-    <col customWidth="1" max="14" min="14" width="6"/>
-    <col customWidth="1" max="15" min="15" width="6"/>
-    <col customWidth="1" max="16" min="16" width="12"/>
-    <col customWidth="1" max="17" min="17" width="17"/>
-    <col customWidth="1" max="18" min="18" width="27"/>
-    <col customWidth="1" max="19" min="19" width="18"/>
-    <col customWidth="1" max="20" min="20" width="18"/>
-    <col customWidth="1" max="21" min="21" width="27"/>
-    <col customWidth="1" max="22" min="22" width="12"/>
-    <col customWidth="1" max="23" min="23" width="12"/>
+    <col customWidth="1" max="13" min="13" width="11"/>
+    <col customWidth="1" max="14" min="14" width="14"/>
+    <col customWidth="1" max="15" min="15" width="12"/>
+    <col customWidth="1" max="16" min="16" width="16"/>
+    <col customWidth="1" max="17" min="17" width="11"/>
+    <col customWidth="1" max="18" min="18" width="11"/>
+    <col customWidth="1" max="19" min="19" width="14"/>
+    <col customWidth="1" max="20" min="20" width="12"/>
+    <col customWidth="1" max="21" min="21" width="16"/>
+    <col customWidth="1" max="22" min="22" width="11"/>
+    <col customWidth="1" max="23" min="23" width="8"/>
+    <col customWidth="1" max="24" min="24" width="6"/>
+    <col customWidth="1" max="25" min="25" width="6"/>
+    <col customWidth="1" max="26" min="26" width="11"/>
+    <col customWidth="1" max="27" min="27" width="14"/>
+    <col customWidth="1" max="28" min="28" width="12"/>
+    <col customWidth="1" max="29" min="29" width="16"/>
+    <col customWidth="1" max="30" min="30" width="11"/>
+    <col customWidth="1" max="31" min="31" width="17"/>
+    <col customWidth="1" max="32" min="32" width="27"/>
+    <col customWidth="1" max="33" min="33" width="18"/>
+    <col customWidth="1" max="34" min="34" width="18"/>
+    <col customWidth="1" max="35" min="35" width="27"/>
+    <col customWidth="1" max="36" min="36" width="12"/>
+    <col customWidth="1" max="37" min="37" width="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:37">
       <c r="A1" t="s">
         <v>221</v>
       </c>
@@ -1946,25 +1988,67 @@
         <v>266</v>
       </c>
       <c r="R1" t="s">
+        <v>262</v>
+      </c>
+      <c r="S1" t="s">
+        <v>263</v>
+      </c>
+      <c r="T1" t="s">
+        <v>264</v>
+      </c>
+      <c r="U1" t="s">
+        <v>265</v>
+      </c>
+      <c r="V1" t="s">
+        <v>266</v>
+      </c>
+      <c r="W1" t="s">
+        <v>267</v>
+      </c>
+      <c r="X1" t="s">
+        <v>268</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>269</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>262</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>264</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>265</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>266</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>270</v>
+      </c>
+      <c r="AF1" t="s">
         <v>256</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AG1" t="s">
         <v>257</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AH1" t="s">
         <v>258</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AI1" t="s">
         <v>259</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AJ1" t="s">
         <v>227</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AK1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:37">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
@@ -1983,25 +2067,69 @@
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
       <c r="L2" s="1" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="N2" s="1" t="n"/>
-      <c r="O2" s="1" t="n"/>
+        <v>272</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="P2" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="Q2" s="1" t="n"/>
-      <c r="R2" s="1" t="n"/>
-      <c r="S2" s="1" t="n"/>
-      <c r="T2" s="1" t="n"/>
-      <c r="U2" s="1" t="n"/>
-      <c r="V2" s="1" t="n"/>
-      <c r="W2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:23">
+        <v>275</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="X2" s="1" t="n"/>
+      <c r="Y2" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="AE2" s="1" t="n"/>
+      <c r="AF2" s="1" t="n"/>
+      <c r="AG2" s="1" t="n"/>
+      <c r="AH2" s="1" t="n"/>
+      <c r="AI2" s="1" t="n"/>
+      <c r="AJ2" s="1" t="n"/>
+      <c r="AK2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:37">
       <c r="A3" s="2" t="s">
         <v>233</v>
       </c>
@@ -2021,54 +2149,96 @@
         <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>277</v>
+        <v>207</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>282</v>
+        <v>207</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="V3" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>290</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="AH3" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="AI3" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="AJ3" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="AK3" s="2" t="s">
         <v>241</v>
       </c>
     </row>
@@ -2083,7 +2253,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2102,11 +2272,16 @@
     <col customWidth="1" max="9" min="9" width="12"/>
     <col customWidth="1" max="10" min="10" width="16"/>
     <col customWidth="1" max="11" min="11" width="9"/>
-    <col customWidth="1" max="12" min="12" width="12"/>
-    <col customWidth="1" max="13" min="13" width="12"/>
+    <col customWidth="1" max="12" min="12" width="13"/>
+    <col customWidth="1" max="13" min="13" width="9"/>
+    <col customWidth="1" max="14" min="14" width="8"/>
+    <col customWidth="1" max="15" min="15" width="11"/>
+    <col customWidth="1" max="16" min="16" width="12"/>
+    <col customWidth="1" max="17" min="17" width="12"/>
+    <col customWidth="1" max="18" min="18" width="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>221</v>
       </c>
@@ -2126,28 +2301,43 @@
         <v>226</v>
       </c>
       <c r="G1" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="H1" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="I1" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="J1" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="K1" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="L1" t="s">
+        <v>302</v>
+      </c>
+      <c r="M1" t="s">
+        <v>303</v>
+      </c>
+      <c r="N1" t="s">
+        <v>304</v>
+      </c>
+      <c r="O1" t="s">
+        <v>305</v>
+      </c>
+      <c r="P1" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q1" t="s">
         <v>227</v>
       </c>
-      <c r="M1" t="s">
+      <c r="R1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="n"/>
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
@@ -2161,16 +2351,23 @@
         <v>232</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>290</v>
+        <v>307</v>
       </c>
       <c r="H2" s="1" t="n"/>
-      <c r="I2" s="1" t="n"/>
+      <c r="I2" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
       <c r="L2" s="1" t="n"/>
       <c r="M2" s="1" t="n"/>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" s="1" t="n"/>
+      <c r="O2" s="1" t="n"/>
+      <c r="P2" s="1" t="n"/>
+      <c r="Q2" s="1" t="n"/>
+      <c r="R2" s="1" t="n"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="2" t="s">
         <v>233</v>
       </c>
@@ -2190,24 +2387,39 @@
         <v>238</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>241</v>
       </c>
     </row>
@@ -2240,57 +2452,57 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>296</v>
+        <v>262</v>
       </c>
       <c r="B1" t="s">
-        <v>297</v>
+        <v>263</v>
       </c>
       <c r="C1" t="s">
-        <v>298</v>
+        <v>264</v>
       </c>
       <c r="D1" t="s">
-        <v>299</v>
+        <v>265</v>
       </c>
       <c r="E1" t="s">
-        <v>300</v>
+        <v>266</v>
       </c>
       <c r="F1" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>302</v>
+        <v>272</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>303</v>
+        <v>273</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>304</v>
+        <v>274</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>305</v>
+        <v>275</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>306</v>
+        <v>276</v>
       </c>
       <c r="F2" s="1" t="n"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>207</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>310</v>
+        <v>288</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>233</v>
@@ -2326,25 +2538,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="B1" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="C1" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="D1" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="E1" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="F1" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="G1" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2352,35 +2564,35 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="F2" s="1" t="n"/>
       <c r="G2" s="1" t="n"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -2414,28 +2626,28 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
       <c r="B1" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="C1" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="D1" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="E1" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="F1" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="G1" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="H1" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2443,7 +2655,7 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -2456,28 +2668,28 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>93</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -2677,7 +2889,7 @@
     <col customWidth="1" max="2" min="2" width="16"/>
     <col customWidth="1" max="3" min="3" width="23"/>
     <col customWidth="1" max="4" min="4" width="13"/>
-    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="5" min="5" width="20"/>
     <col customWidth="1" max="6" min="6" width="8"/>
     <col customWidth="1" max="7" min="7" width="9"/>
     <col customWidth="1" max="8" min="8" width="19"/>
@@ -3073,7 +3285,7 @@
     <col customWidth="1" max="2" min="2" width="16"/>
     <col customWidth="1" max="3" min="3" width="23"/>
     <col customWidth="1" max="4" min="4" width="13"/>
-    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="5" min="5" width="20"/>
     <col customWidth="1" max="6" min="6" width="8"/>
     <col customWidth="1" max="7" min="7" width="9"/>
     <col customWidth="1" max="8" min="8" width="19"/>
@@ -3334,7 +3546,7 @@
     <col customWidth="1" max="2" min="2" width="16"/>
     <col customWidth="1" max="3" min="3" width="23"/>
     <col customWidth="1" max="4" min="4" width="13"/>
-    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="5" min="5" width="20"/>
     <col customWidth="1" max="6" min="6" width="8"/>
     <col customWidth="1" max="7" min="7" width="9"/>
     <col customWidth="1" max="8" min="8" width="19"/>
@@ -3571,7 +3783,7 @@
     <col customWidth="1" max="2" min="2" width="16"/>
     <col customWidth="1" max="3" min="3" width="23"/>
     <col customWidth="1" max="4" min="4" width="13"/>
-    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="5" min="5" width="20"/>
     <col customWidth="1" max="6" min="6" width="8"/>
     <col customWidth="1" max="7" min="7" width="9"/>
     <col customWidth="1" max="8" min="8" width="19"/>
@@ -3848,7 +4060,7 @@
     <col customWidth="1" max="2" min="2" width="16"/>
     <col customWidth="1" max="3" min="3" width="23"/>
     <col customWidth="1" max="4" min="4" width="13"/>
-    <col customWidth="1" max="5" min="5" width="12"/>
+    <col customWidth="1" max="5" min="5" width="20"/>
     <col customWidth="1" max="6" min="6" width="8"/>
     <col customWidth="1" max="7" min="7" width="9"/>
     <col customWidth="1" max="8" min="8" width="19"/>

</xml_diff>

<commit_message>
Updated json to spreadsheet script to use local file and concatenate concept-module field name for integrated names if user friendly available. Updated library_preparation_process.json to work with this
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/v5/template/Programmatically_generated_v5_template_spreadsheet.xlsx
+++ b/examples/spreadsheets/v5/template/Programmatically_generated_v5_template_spreadsheet.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="366">
   <si>
     <t>A unique label for the project.</t>
   </si>
@@ -589,37 +589,37 @@
     <t>100 ug/mL ampicillin</t>
   </si>
   <si>
-    <t>Cell morphology</t>
-  </si>
-  <si>
-    <t>Cell size number</t>
-  </si>
-  <si>
-    <t>Cell size unit</t>
-  </si>
-  <si>
-    <t>Percent cell viability</t>
-  </si>
-  <si>
-    <t>Cell viability method</t>
-  </si>
-  <si>
-    <t>Percent necrosis</t>
-  </si>
-  <si>
-    <t>Passage number</t>
-  </si>
-  <si>
-    <t>Growth medium</t>
-  </si>
-  <si>
-    <t>Mycoplasma testing method</t>
-  </si>
-  <si>
-    <t>Mycoplasma testing results</t>
-  </si>
-  <si>
-    <t>Drug treatment</t>
+    <t>Cell morphology - Cell morphology</t>
+  </si>
+  <si>
+    <t>Cell morphology - Cell size number</t>
+  </si>
+  <si>
+    <t>Cell morphology - Cell size unit</t>
+  </si>
+  <si>
+    <t>Cell morphology - Percent cell viability</t>
+  </si>
+  <si>
+    <t>Cell morphology - Cell viability method</t>
+  </si>
+  <si>
+    <t>Cell morphology - Percent necrosis</t>
+  </si>
+  <si>
+    <t>Growth conditions - Passage number</t>
+  </si>
+  <si>
+    <t>Growth conditions - Growth medium</t>
+  </si>
+  <si>
+    <t>Growth conditions - Mycoplasma testing method</t>
+  </si>
+  <si>
+    <t>Growth conditions - Mycoplasma testing results</t>
+  </si>
+  <si>
+    <t>Growth conditions - Drug treatment</t>
   </si>
   <si>
     <t>Target cell type</t>
@@ -868,16 +868,16 @@
     <t>unstranded</t>
   </si>
   <si>
-    <t>Cell Barcode-containing read</t>
-  </si>
-  <si>
-    <t>Cell Barcode offset</t>
-  </si>
-  <si>
-    <t>Cell Barcode length</t>
-  </si>
-  <si>
-    <t>Cell White list barcode file</t>
+    <t>Cell barcode - Barcode-containing read</t>
+  </si>
+  <si>
+    <t>Cell barcode - Barcode offset</t>
+  </si>
+  <si>
+    <t>Cell barcode - Barcode length</t>
+  </si>
+  <si>
+    <t>Cell barcode - White list barcode file</t>
   </si>
   <si>
     <t>Input nucleic acid molecule</t>
@@ -886,6 +886,138 @@
     <t>Library construction approach</t>
   </si>
   <si>
+    <t>Library construction kit - Retail name</t>
+  </si>
+  <si>
+    <t>Library construction kit - Catalog number</t>
+  </si>
+  <si>
+    <t>Library construction kit - Manufacturer</t>
+  </si>
+  <si>
+    <t>Library construction kit - Batch/lot number</t>
+  </si>
+  <si>
+    <t>Library construction kit - Expiry date</t>
+  </si>
+  <si>
+    <t>Nucleic acid conversion kit - Retail name</t>
+  </si>
+  <si>
+    <t>Nucleic acid conversion kit - Catalog number</t>
+  </si>
+  <si>
+    <t>Nucleic acid conversion kit - Manufacturer</t>
+  </si>
+  <si>
+    <t>Nucleic acid conversion kit - Batch/lot number</t>
+  </si>
+  <si>
+    <t>Nucleic acid conversion kit - Expiry date</t>
+  </si>
+  <si>
+    <t>End bias</t>
+  </si>
+  <si>
+    <t>Primer</t>
+  </si>
+  <si>
+    <t>Strand</t>
+  </si>
+  <si>
+    <t>Spike-in kit - Retail name</t>
+  </si>
+  <si>
+    <t>Spike-in kit - Catalog number</t>
+  </si>
+  <si>
+    <t>Spike-in kit - Manufacturer</t>
+  </si>
+  <si>
+    <t>Spike-in kit - Batch/lot number</t>
+  </si>
+  <si>
+    <t>Spike-in kit - Expiry date</t>
+  </si>
+  <si>
+    <t>Spike-in dilution</t>
+  </si>
+  <si>
+    <t>UMI barcode - Barcode-containing read</t>
+  </si>
+  <si>
+    <t>UMI barcode - Barcode offset</t>
+  </si>
+  <si>
+    <t>UMI barcode - Barcode length</t>
+  </si>
+  <si>
+    <t>UMI barcode - White list barcode file</t>
+  </si>
+  <si>
+    <t>The manufacturer and model of the sequencer used. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/efo/terms?iri=http%3A%2F%2Fwww.ebi.ac.uk%2Fefo%2FEFO_0000548.</t>
+  </si>
+  <si>
+    <t>Local name for the particular machine on which the biomaterial was sequenced.</t>
+  </si>
+  <si>
+    <t>Was a paired-end sequencing strategy used? Must be either yes or no.</t>
+  </si>
+  <si>
+    <t>An INSDC (International Nucleotide Sequence Database Collaboration) experiment accession. Accession must start with DRX, ERX, or SRX.</t>
+  </si>
+  <si>
+    <t>An ID for the plate that the well is located on.</t>
+  </si>
+  <si>
+    <t>A name for the well. Should be unique for the plate</t>
+  </si>
+  <si>
+    <t>Well row in plate.</t>
+  </si>
+  <si>
+    <t>Well column in plate.</t>
+  </si>
+  <si>
+    <t>Note on how good cell looks if imaged in well before sequencing.</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 4000</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>Instrument manufacturer and model</t>
+  </si>
+  <si>
+    <t>Local machine name</t>
+  </si>
+  <si>
+    <t>Paired ends?</t>
+  </si>
+  <si>
+    <t>INSDC experiment</t>
+  </si>
+  <si>
+    <t>Well plate ID</t>
+  </si>
+  <si>
+    <t>Well name</t>
+  </si>
+  <si>
+    <t>Well row</t>
+  </si>
+  <si>
+    <t>Well column</t>
+  </si>
+  <si>
+    <t>Cell quality</t>
+  </si>
+  <si>
+    <t>ID for process this purchased_reagents relates to</t>
+  </si>
+  <si>
     <t>Retail name</t>
   </si>
   <si>
@@ -896,93 +1028,6 @@
   </si>
   <si>
     <t>Expiry date</t>
-  </si>
-  <si>
-    <t>End bias</t>
-  </si>
-  <si>
-    <t>Primer</t>
-  </si>
-  <si>
-    <t>Strand</t>
-  </si>
-  <si>
-    <t>Spike-in dilution</t>
-  </si>
-  <si>
-    <t>UMI Barcode-containing read</t>
-  </si>
-  <si>
-    <t>UMI Barcode offset</t>
-  </si>
-  <si>
-    <t>UMI Barcode length</t>
-  </si>
-  <si>
-    <t>UMI White list barcode file</t>
-  </si>
-  <si>
-    <t>The manufacturer and model of the sequencer used. Should be a child term of https://www.ebi.ac.uk/ols/ontologies/efo/terms?iri=http%3A%2F%2Fwww.ebi.ac.uk%2Fefo%2FEFO_0000548.</t>
-  </si>
-  <si>
-    <t>Local name for the particular machine on which the biomaterial was sequenced.</t>
-  </si>
-  <si>
-    <t>Was a paired-end sequencing strategy used? Must be either yes or no.</t>
-  </si>
-  <si>
-    <t>An INSDC (International Nucleotide Sequence Database Collaboration) experiment accession. Accession must start with DRX, ERX, or SRX.</t>
-  </si>
-  <si>
-    <t>An ID for the plate that the well is located on.</t>
-  </si>
-  <si>
-    <t>A name for the well. Should be unique for the plate</t>
-  </si>
-  <si>
-    <t>Well row in plate.</t>
-  </si>
-  <si>
-    <t>Well column in plate.</t>
-  </si>
-  <si>
-    <t>Note on how good cell looks if imaged in well before sequencing.</t>
-  </si>
-  <si>
-    <t>Illumina HiSeq 4000</t>
-  </si>
-  <si>
-    <t>yes</t>
-  </si>
-  <si>
-    <t>Instrument manufacturer and model</t>
-  </si>
-  <si>
-    <t>Local machine name</t>
-  </si>
-  <si>
-    <t>Paired ends?</t>
-  </si>
-  <si>
-    <t>INSDC experiment</t>
-  </si>
-  <si>
-    <t>Well plate ID</t>
-  </si>
-  <si>
-    <t>Well name</t>
-  </si>
-  <si>
-    <t>Well row</t>
-  </si>
-  <si>
-    <t>Well column</t>
-  </si>
-  <si>
-    <t>Cell quality</t>
-  </si>
-  <si>
-    <t>ID for process this purchased_reagents relates to</t>
   </si>
   <si>
     <t>A unique ID for this protocol.</t>
@@ -1545,17 +1590,17 @@
     <col customWidth="1" max="8" min="8" width="19"/>
     <col customWidth="1" max="9" min="9" width="12"/>
     <col customWidth="1" max="10" min="10" width="8"/>
-    <col customWidth="1" max="11" min="11" width="15"/>
-    <col customWidth="1" max="12" min="12" width="16"/>
-    <col customWidth="1" max="13" min="13" width="14"/>
-    <col customWidth="1" max="14" min="14" width="22"/>
-    <col customWidth="1" max="15" min="15" width="21"/>
-    <col customWidth="1" max="16" min="16" width="16"/>
-    <col customWidth="1" max="17" min="17" width="14"/>
-    <col customWidth="1" max="18" min="18" width="13"/>
-    <col customWidth="1" max="19" min="19" width="25"/>
-    <col customWidth="1" max="20" min="20" width="26"/>
-    <col customWidth="1" max="21" min="21" width="14"/>
+    <col customWidth="1" max="11" min="11" width="33"/>
+    <col customWidth="1" max="12" min="12" width="34"/>
+    <col customWidth="1" max="13" min="13" width="32"/>
+    <col customWidth="1" max="14" min="14" width="40"/>
+    <col customWidth="1" max="15" min="15" width="39"/>
+    <col customWidth="1" max="16" min="16" width="34"/>
+    <col customWidth="1" max="17" min="17" width="34"/>
+    <col customWidth="1" max="18" min="18" width="33"/>
+    <col customWidth="1" max="19" min="19" width="45"/>
+    <col customWidth="1" max="20" min="20" width="46"/>
+    <col customWidth="1" max="21" min="21" width="34"/>
     <col customWidth="1" max="22" min="22" width="13"/>
     <col customWidth="1" max="23" min="23" width="11"/>
     <col customWidth="1" max="24" min="24" width="12"/>
@@ -2147,35 +2192,35 @@
     <col customWidth="1" max="4" min="4" width="10"/>
     <col customWidth="1" max="5" min="5" width="8"/>
     <col customWidth="1" max="6" min="6" width="17"/>
-    <col customWidth="1" max="7" min="7" width="28"/>
-    <col customWidth="1" max="8" min="8" width="19"/>
-    <col customWidth="1" max="9" min="9" width="19"/>
-    <col customWidth="1" max="10" min="10" width="28"/>
+    <col customWidth="1" max="7" min="7" width="38"/>
+    <col customWidth="1" max="8" min="8" width="29"/>
+    <col customWidth="1" max="9" min="9" width="29"/>
+    <col customWidth="1" max="10" min="10" width="38"/>
     <col customWidth="1" max="11" min="11" width="27"/>
     <col customWidth="1" max="12" min="12" width="29"/>
-    <col customWidth="1" max="13" min="13" width="11"/>
-    <col customWidth="1" max="14" min="14" width="14"/>
-    <col customWidth="1" max="15" min="15" width="12"/>
-    <col customWidth="1" max="16" min="16" width="16"/>
-    <col customWidth="1" max="17" min="17" width="11"/>
-    <col customWidth="1" max="18" min="18" width="11"/>
-    <col customWidth="1" max="19" min="19" width="14"/>
-    <col customWidth="1" max="20" min="20" width="12"/>
-    <col customWidth="1" max="21" min="21" width="16"/>
-    <col customWidth="1" max="22" min="22" width="11"/>
+    <col customWidth="1" max="13" min="13" width="38"/>
+    <col customWidth="1" max="14" min="14" width="41"/>
+    <col customWidth="1" max="15" min="15" width="39"/>
+    <col customWidth="1" max="16" min="16" width="43"/>
+    <col customWidth="1" max="17" min="17" width="38"/>
+    <col customWidth="1" max="18" min="18" width="41"/>
+    <col customWidth="1" max="19" min="19" width="44"/>
+    <col customWidth="1" max="20" min="20" width="42"/>
+    <col customWidth="1" max="21" min="21" width="46"/>
+    <col customWidth="1" max="22" min="22" width="41"/>
     <col customWidth="1" max="23" min="23" width="8"/>
     <col customWidth="1" max="24" min="24" width="6"/>
     <col customWidth="1" max="25" min="25" width="6"/>
-    <col customWidth="1" max="26" min="26" width="11"/>
-    <col customWidth="1" max="27" min="27" width="14"/>
-    <col customWidth="1" max="28" min="28" width="12"/>
-    <col customWidth="1" max="29" min="29" width="16"/>
-    <col customWidth="1" max="30" min="30" width="11"/>
+    <col customWidth="1" max="26" min="26" width="26"/>
+    <col customWidth="1" max="27" min="27" width="29"/>
+    <col customWidth="1" max="28" min="28" width="27"/>
+    <col customWidth="1" max="29" min="29" width="31"/>
+    <col customWidth="1" max="30" min="30" width="26"/>
     <col customWidth="1" max="31" min="31" width="17"/>
-    <col customWidth="1" max="32" min="32" width="27"/>
-    <col customWidth="1" max="33" min="33" width="18"/>
-    <col customWidth="1" max="34" min="34" width="18"/>
-    <col customWidth="1" max="35" min="35" width="27"/>
+    <col customWidth="1" max="32" min="32" width="37"/>
+    <col customWidth="1" max="33" min="33" width="28"/>
+    <col customWidth="1" max="34" min="34" width="28"/>
+    <col customWidth="1" max="35" min="35" width="37"/>
     <col customWidth="1" max="36" min="36" width="12"/>
     <col customWidth="1" max="37" min="37" width="12"/>
   </cols>
@@ -2415,70 +2460,70 @@
         <v>284</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>205</v>
+        <v>285</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>205</v>
+        <v>290</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>284</v>
+        <v>297</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>205</v>
+        <v>298</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>285</v>
+        <v>299</v>
       </c>
       <c r="AC3" s="2" t="s">
-        <v>286</v>
+        <v>300</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>291</v>
+        <v>302</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>292</v>
+        <v>303</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="AI3" s="2" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="AJ3" s="2" t="s">
         <v>238</v>
@@ -2545,31 +2590,31 @@
         <v>225</v>
       </c>
       <c r="G1" t="s">
-        <v>296</v>
+        <v>307</v>
       </c>
       <c r="H1" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="I1" t="s">
-        <v>298</v>
+        <v>309</v>
       </c>
       <c r="J1" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="K1" t="s">
-        <v>300</v>
+        <v>311</v>
       </c>
       <c r="L1" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="M1" t="s">
-        <v>302</v>
+        <v>313</v>
       </c>
       <c r="N1" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="O1" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="P1" t="s">
         <v>226</v>
@@ -2592,11 +2637,11 @@
         <v>231</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>305</v>
+        <v>316</v>
       </c>
       <c r="H2" s="1" t="n"/>
       <c r="I2" s="1" t="s">
-        <v>306</v>
+        <v>317</v>
       </c>
       <c r="J2" s="1" t="n"/>
       <c r="K2" s="1" t="n"/>
@@ -2627,31 +2672,31 @@
         <v>237</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>307</v>
+        <v>318</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>308</v>
+        <v>319</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>309</v>
+        <v>320</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>311</v>
+        <v>322</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>238</v>
@@ -2704,7 +2749,7 @@
         <v>265</v>
       </c>
       <c r="F1" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2727,19 +2772,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>284</v>
+        <v>328</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>205</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>285</v>
+        <v>329</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>286</v>
+        <v>330</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>287</v>
+        <v>331</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>232</v>
@@ -2775,25 +2820,25 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="B1" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="C1" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="D1" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="E1" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
       <c r="F1" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="G1" t="s">
-        <v>323</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2801,35 +2846,35 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="F2" s="1" t="n"/>
       <c r="G2" s="1" t="n"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>329</v>
+        <v>344</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>332</v>
+        <v>347</v>
       </c>
     </row>
   </sheetData>
@@ -2864,31 +2909,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="B1" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
       <c r="C1" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="D1" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
       <c r="E1" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="F1" t="s">
-        <v>338</v>
+        <v>353</v>
       </c>
       <c r="G1" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
       <c r="H1" t="s">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="I1" t="s">
-        <v>341</v>
+        <v>356</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -2896,7 +2941,7 @@
       <c r="B2" s="1" t="n"/>
       <c r="C2" s="1" t="n"/>
       <c r="D2" s="1" t="s">
-        <v>342</v>
+        <v>357</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
@@ -2910,31 +2955,31 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>343</v>
+        <v>358</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>344</v>
+        <v>359</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>345</v>
+        <v>360</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>346</v>
+        <v>361</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>347</v>
+        <v>362</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>348</v>
+        <v>363</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>349</v>
+        <v>364</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>91</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>350</v>
+        <v>365</v>
       </c>
     </row>
   </sheetData>
@@ -3797,17 +3842,17 @@
     <col customWidth="1" max="8" min="8" width="19"/>
     <col customWidth="1" max="9" min="9" width="12"/>
     <col customWidth="1" max="10" min="10" width="8"/>
-    <col customWidth="1" max="11" min="11" width="15"/>
-    <col customWidth="1" max="12" min="12" width="16"/>
-    <col customWidth="1" max="13" min="13" width="14"/>
-    <col customWidth="1" max="14" min="14" width="22"/>
-    <col customWidth="1" max="15" min="15" width="21"/>
-    <col customWidth="1" max="16" min="16" width="16"/>
-    <col customWidth="1" max="17" min="17" width="14"/>
-    <col customWidth="1" max="18" min="18" width="13"/>
-    <col customWidth="1" max="19" min="19" width="25"/>
-    <col customWidth="1" max="20" min="20" width="26"/>
-    <col customWidth="1" max="21" min="21" width="14"/>
+    <col customWidth="1" max="11" min="11" width="33"/>
+    <col customWidth="1" max="12" min="12" width="34"/>
+    <col customWidth="1" max="13" min="13" width="32"/>
+    <col customWidth="1" max="14" min="14" width="40"/>
+    <col customWidth="1" max="15" min="15" width="39"/>
+    <col customWidth="1" max="16" min="16" width="34"/>
+    <col customWidth="1" max="17" min="17" width="34"/>
+    <col customWidth="1" max="18" min="18" width="33"/>
+    <col customWidth="1" max="19" min="19" width="45"/>
+    <col customWidth="1" max="20" min="20" width="46"/>
+    <col customWidth="1" max="21" min="21" width="34"/>
     <col customWidth="1" max="22" min="22" width="13"/>
     <col customWidth="1" max="23" min="23" width="16"/>
     <col customWidth="1" max="24" min="24" width="26"/>
@@ -4038,17 +4083,17 @@
     <col customWidth="1" max="12" min="12" width="11"/>
     <col customWidth="1" max="13" min="13" width="10"/>
     <col customWidth="1" max="14" min="14" width="14"/>
-    <col customWidth="1" max="15" min="15" width="15"/>
-    <col customWidth="1" max="16" min="16" width="16"/>
-    <col customWidth="1" max="17" min="17" width="14"/>
-    <col customWidth="1" max="18" min="18" width="22"/>
-    <col customWidth="1" max="19" min="19" width="21"/>
-    <col customWidth="1" max="20" min="20" width="16"/>
-    <col customWidth="1" max="21" min="21" width="14"/>
-    <col customWidth="1" max="22" min="22" width="13"/>
-    <col customWidth="1" max="23" min="23" width="25"/>
-    <col customWidth="1" max="24" min="24" width="26"/>
-    <col customWidth="1" max="25" min="25" width="14"/>
+    <col customWidth="1" max="15" min="15" width="33"/>
+    <col customWidth="1" max="16" min="16" width="34"/>
+    <col customWidth="1" max="17" min="17" width="32"/>
+    <col customWidth="1" max="18" min="18" width="40"/>
+    <col customWidth="1" max="19" min="19" width="39"/>
+    <col customWidth="1" max="20" min="20" width="34"/>
+    <col customWidth="1" max="21" min="21" width="34"/>
+    <col customWidth="1" max="22" min="22" width="33"/>
+    <col customWidth="1" max="23" min="23" width="45"/>
+    <col customWidth="1" max="24" min="24" width="46"/>
+    <col customWidth="1" max="25" min="25" width="34"/>
     <col customWidth="1" max="26" min="26" width="9"/>
     <col customWidth="1" max="27" min="27" width="16"/>
     <col customWidth="1" max="28" min="28" width="7"/>

</xml_diff>